<commit_message>
correct .xlsx file and dependencies
</commit_message>
<xml_diff>
--- a/relchange.xlsx
+++ b/relchange.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxku\OneDrive\Documents\Silas\Silas_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D6B54091-1436-4A8F-BBD3-482E2E0D1204}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B20824-C097-46DB-8B34-D67B52327DE8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="relchange" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -79,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -914,11 +922,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2392" workbookViewId="0">
-      <selection activeCell="F2238" sqref="F2238:F2409"/>
+    <sheetView tabSelected="1" topLeftCell="A2615" workbookViewId="0">
+      <selection activeCell="F346" sqref="F346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,7 +965,8 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>D2/$D$2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>